<commit_message>
added BABIP expectation to draft guide to show expected regression or improvement
</commit_message>
<xml_diff>
--- a/yearly_draft_guides/fantasy_baseball_draft_tool_2025.xlsx
+++ b/yearly_draft_guides/fantasy_baseball_draft_tool_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212445956\Desktop\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE2DEAB1-48AC-4ECD-8DFD-70A77BF0354F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9883EA91-1B57-4514-91D4-DFAB0D782D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{617A30E1-45C1-45FD-9B14-2C512446505A}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="ADP" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ideal_Lineup!$A$31:$E$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ideal_Lineup!$A$31:$G$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4041" uniqueCount="1410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4131" uniqueCount="1413">
   <si>
     <t>Tier 1</t>
   </si>
@@ -4294,6 +4294,15 @@
   </si>
   <si>
     <t>Position</t>
+  </si>
+  <si>
+    <t>BABIP_Expectation_Batter</t>
+  </si>
+  <si>
+    <t>BABIP_Expectation_Pitcher</t>
+  </si>
+  <si>
+    <t>Regression</t>
   </si>
 </sst>
 </file>
@@ -4797,10 +4806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B159E54-99E5-4537-A261-1352C227AF32}">
-  <dimension ref="A1:E213"/>
+  <dimension ref="A1:H213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4809,6 +4818,8 @@
     <col min="2" max="2" width="22.26953125" customWidth="1"/>
     <col min="3" max="3" width="20.08984375" customWidth="1"/>
     <col min="4" max="4" width="17.76953125" customWidth="1"/>
+    <col min="6" max="6" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.40625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.75">
@@ -5035,7 +5046,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5049,7 +5060,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5063,7 +5074,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5077,7 +5088,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5091,7 +5102,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5105,7 +5116,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5119,7 +5130,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5133,7 +5144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5147,7 +5158,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5161,7 +5172,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A31" s="1" t="s">
         <v>187</v>
       </c>
@@ -5177,8 +5188,15 @@
       <c r="E31" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F31" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>1411</v>
+      </c>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -5194,8 +5212,14 @@
       <c r="E32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -5211,8 +5235,14 @@
       <c r="E33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F33" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G33" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -5228,8 +5258,14 @@
       <c r="E34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F34" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G34" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>239</v>
       </c>
@@ -5245,8 +5281,14 @@
       <c r="E35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
         <v>238</v>
       </c>
@@ -5262,8 +5304,14 @@
       <c r="E36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -5279,8 +5327,14 @@
       <c r="E37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -5296,8 +5350,14 @@
       <c r="E38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F38" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G38" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -5313,8 +5373,14 @@
       <c r="E39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F39" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -5330,8 +5396,14 @@
       <c r="E40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F40" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>198</v>
       </c>
@@ -5347,8 +5419,14 @@
       <c r="E41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F41" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G41" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>952</v>
       </c>
@@ -5364,8 +5442,14 @@
       <c r="E42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G42" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -5381,8 +5465,14 @@
       <c r="E43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
         <v>210</v>
       </c>
@@ -5398,8 +5488,14 @@
       <c r="E44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>949</v>
       </c>
@@ -5415,8 +5511,14 @@
       <c r="E45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -5432,8 +5534,14 @@
       <c r="E46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F46" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -5449,8 +5557,14 @@
       <c r="E47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
         <v>209</v>
       </c>
@@ -5466,8 +5580,14 @@
       <c r="E48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F48" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -5483,8 +5603,14 @@
       <c r="E49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
         <v>950</v>
       </c>
@@ -5500,8 +5626,14 @@
       <c r="E50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G50" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A51" t="s">
         <v>324</v>
       </c>
@@ -5517,8 +5649,14 @@
       <c r="E51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F51" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -5534,8 +5672,14 @@
       <c r="E52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F52" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -5551,8 +5695,14 @@
       <c r="E53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F53" t="s">
+        <v>6</v>
+      </c>
+      <c r="G53" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A54" t="s">
         <v>268</v>
       </c>
@@ -5568,8 +5718,14 @@
       <c r="E54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F54" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G54" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A55" t="s">
         <v>27</v>
       </c>
@@ -5585,8 +5741,14 @@
       <c r="E55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A56" t="s">
         <v>330</v>
       </c>
@@ -5602,8 +5764,14 @@
       <c r="E56">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F56" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A57" t="s">
         <v>953</v>
       </c>
@@ -5619,8 +5787,14 @@
       <c r="E57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F57" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G57" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A58" t="s">
         <v>200</v>
       </c>
@@ -5636,8 +5810,14 @@
       <c r="E58">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F58" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A59" t="s">
         <v>32</v>
       </c>
@@ -5653,8 +5833,14 @@
       <c r="E59">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F59" t="s">
+        <v>6</v>
+      </c>
+      <c r="G59" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A60" t="s">
         <v>199</v>
       </c>
@@ -5670,8 +5856,14 @@
       <c r="E60">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F60" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A61" t="s">
         <v>955</v>
       </c>
@@ -5687,8 +5879,14 @@
       <c r="E61">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F61" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G61" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
         <v>951</v>
       </c>
@@ -5704,8 +5902,14 @@
       <c r="E62">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F62" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G62" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A63" t="s">
         <v>208</v>
       </c>
@@ -5721,8 +5925,14 @@
       <c r="E63">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F63" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A64" t="s">
         <v>216</v>
       </c>
@@ -5738,8 +5948,14 @@
       <c r="E64">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F64" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A65" t="s">
         <v>207</v>
       </c>
@@ -5755,8 +5971,14 @@
       <c r="E65">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F65" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A66" t="s">
         <v>958</v>
       </c>
@@ -5772,8 +5994,14 @@
       <c r="E66">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F66" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G66" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A67" t="s">
         <v>217</v>
       </c>
@@ -5789,8 +6017,14 @@
       <c r="E67">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F67" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G67" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A68" t="s">
         <v>994</v>
       </c>
@@ -5806,8 +6040,14 @@
       <c r="E68">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F68" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G68" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A69" t="s">
         <v>221</v>
       </c>
@@ -5823,8 +6063,14 @@
       <c r="E69">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F69" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A70" t="s">
         <v>987</v>
       </c>
@@ -5840,8 +6086,14 @@
       <c r="E70">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F70" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G70" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A71" t="s">
         <v>269</v>
       </c>
@@ -5857,8 +6109,14 @@
       <c r="E71">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F71" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A72" t="s">
         <v>959</v>
       </c>
@@ -5874,8 +6132,14 @@
       <c r="E72">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F72" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G72" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A73" t="s">
         <v>25</v>
       </c>
@@ -5891,8 +6155,14 @@
       <c r="E73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F73" t="s">
+        <v>6</v>
+      </c>
+      <c r="G73" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A74" t="s">
         <v>964</v>
       </c>
@@ -5908,8 +6178,14 @@
       <c r="E74">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F74" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A75" t="s">
         <v>967</v>
       </c>
@@ -5925,8 +6201,14 @@
       <c r="E75">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F75" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G75" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A76" t="s">
         <v>968</v>
       </c>
@@ -5942,8 +6224,14 @@
       <c r="E76">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F76" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G76" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A77" t="s">
         <v>235</v>
       </c>
@@ -5959,8 +6247,14 @@
       <c r="E77">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F77" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G77" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A78" t="s">
         <v>338</v>
       </c>
@@ -5976,8 +6270,14 @@
       <c r="E78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F78" t="s">
+        <v>6</v>
+      </c>
+      <c r="G78" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A79" t="s">
         <v>339</v>
       </c>
@@ -5993,8 +6293,14 @@
       <c r="E79">
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F79" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G79" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A80" t="s">
         <v>271</v>
       </c>
@@ -6010,8 +6316,14 @@
       <c r="E80">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F80" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A81" t="s">
         <v>983</v>
       </c>
@@ -6027,8 +6339,14 @@
       <c r="E81">
         <v>6</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F81" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -6044,8 +6362,14 @@
       <c r="E82">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F82" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G82" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A83" t="s">
         <v>33</v>
       </c>
@@ -6061,8 +6385,14 @@
       <c r="E83">
         <v>6</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F83" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G83" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A84" t="s">
         <v>215</v>
       </c>
@@ -6078,8 +6408,14 @@
       <c r="E84">
         <v>7</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F84" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G84" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A85" t="s">
         <v>347</v>
       </c>
@@ -6095,8 +6431,14 @@
       <c r="E85">
         <v>7</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F85" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G85" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A86" t="s">
         <v>227</v>
       </c>
@@ -6112,8 +6454,14 @@
       <c r="E86">
         <v>7</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F86" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G86" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A87" t="s">
         <v>954</v>
       </c>
@@ -6129,8 +6477,14 @@
       <c r="E87">
         <v>7</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F87" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G87" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A88" t="s">
         <v>222</v>
       </c>
@@ -6146,8 +6500,14 @@
       <c r="E88">
         <v>7</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F88" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G88" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A89" t="s">
         <v>230</v>
       </c>
@@ -6163,8 +6523,14 @@
       <c r="E89">
         <v>8</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F89" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G89" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A90" t="s">
         <v>970</v>
       </c>
@@ -6180,8 +6546,14 @@
       <c r="E90">
         <v>8</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F90" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A91" t="s">
         <v>206</v>
       </c>
@@ -6197,8 +6569,14 @@
       <c r="E91">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F91" t="s">
+        <v>6</v>
+      </c>
+      <c r="G91" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A92" t="s">
         <v>979</v>
       </c>
@@ -6214,8 +6592,14 @@
       <c r="E92">
         <v>8</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F92" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G92" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A93" t="s">
         <v>205</v>
       </c>
@@ -6231,8 +6615,14 @@
       <c r="E93">
         <v>8</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F93" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G93" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A94" t="s">
         <v>985</v>
       </c>
@@ -6248,8 +6638,14 @@
       <c r="E94">
         <v>8</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F94" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A95" t="s">
         <v>961</v>
       </c>
@@ -6265,8 +6661,14 @@
       <c r="E95">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F95" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G95" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A96" t="s">
         <v>997</v>
       </c>
@@ -6282,8 +6684,14 @@
       <c r="E96">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F96" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A97" t="s">
         <v>252</v>
       </c>
@@ -6299,8 +6707,14 @@
       <c r="E97">
         <v>9</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F97" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G97" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A98" t="s">
         <v>989</v>
       </c>
@@ -6316,8 +6730,14 @@
       <c r="E98">
         <v>9</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F98" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A99" t="s">
         <v>276</v>
       </c>
@@ -6333,8 +6753,14 @@
       <c r="E99">
         <v>9</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F99" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A100" t="s">
         <v>214</v>
       </c>
@@ -6350,8 +6776,14 @@
       <c r="E100">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F100" t="s">
+        <v>15</v>
+      </c>
+      <c r="G100" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A101" t="s">
         <v>219</v>
       </c>
@@ -6367,8 +6799,14 @@
       <c r="E101">
         <v>9</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F101" t="s">
+        <v>15</v>
+      </c>
+      <c r="G101" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A102" t="s">
         <v>254</v>
       </c>
@@ -6384,8 +6822,14 @@
       <c r="E102">
         <v>10</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F102" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A103" t="s">
         <v>363</v>
       </c>
@@ -6401,8 +6845,14 @@
       <c r="E103">
         <v>10</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F103" t="s">
+        <v>6</v>
+      </c>
+      <c r="G103" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A104" t="s">
         <v>224</v>
       </c>
@@ -6418,8 +6868,14 @@
       <c r="E104">
         <v>11</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F104" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G104" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A105" t="s">
         <v>256</v>
       </c>
@@ -6435,8 +6891,14 @@
       <c r="E105">
         <v>11</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F105" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G105" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A106" t="s">
         <v>981</v>
       </c>
@@ -6452,8 +6914,14 @@
       <c r="E106">
         <v>11</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F106" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G106" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A107" t="s">
         <v>203</v>
       </c>
@@ -6469,8 +6937,14 @@
       <c r="E107">
         <v>11</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F107" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G107" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A108" t="s">
         <v>232</v>
       </c>
@@ -6486,8 +6960,14 @@
       <c r="E108">
         <v>11</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F108" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G108" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A109" t="s">
         <v>976</v>
       </c>
@@ -6503,8 +6983,14 @@
       <c r="E109">
         <v>11</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F109" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A110" t="s">
         <v>202</v>
       </c>
@@ -6520,8 +7006,14 @@
       <c r="E110">
         <v>11</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F110" t="s">
+        <v>6</v>
+      </c>
+      <c r="G110" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A111" t="s">
         <v>279</v>
       </c>
@@ -6537,8 +7029,14 @@
       <c r="E111">
         <v>12</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F111" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G111" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A112" t="s">
         <v>376</v>
       </c>
@@ -6554,8 +7052,14 @@
       <c r="E112">
         <v>12</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F112" t="s">
+        <v>15</v>
+      </c>
+      <c r="G112" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A113" t="s">
         <v>960</v>
       </c>
@@ -6571,8 +7075,14 @@
       <c r="E113">
         <v>12</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F113" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G113" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A114" t="s">
         <v>257</v>
       </c>
@@ -6588,8 +7098,14 @@
       <c r="E114">
         <v>12</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F114" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G114" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A115" t="s">
         <v>245</v>
       </c>
@@ -6605,8 +7121,14 @@
       <c r="E115">
         <v>13</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F115" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G115" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A116" t="s">
         <v>963</v>
       </c>
@@ -6622,8 +7144,14 @@
       <c r="E116">
         <v>14</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F116" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G116" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A117" t="s">
         <v>259</v>
       </c>
@@ -6639,8 +7167,14 @@
       <c r="E117">
         <v>14</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F117" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G117" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A118" t="s">
         <v>999</v>
       </c>
@@ -6656,8 +7190,14 @@
       <c r="E118">
         <v>15</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F118" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G118" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A119" t="s">
         <v>966</v>
       </c>
@@ -6673,8 +7213,14 @@
       <c r="E119">
         <v>15</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F119" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G119" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A120" t="s">
         <v>236</v>
       </c>
@@ -6690,8 +7236,14 @@
       <c r="E120">
         <v>15</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F120" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G120" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A121" t="s">
         <v>237</v>
       </c>
@@ -6707,8 +7259,14 @@
       <c r="E121">
         <v>15</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F121" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G121" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A122" t="s">
         <v>400</v>
       </c>
@@ -6724,8 +7282,14 @@
       <c r="E122">
         <v>16</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F122" t="s">
+        <v>6</v>
+      </c>
+      <c r="G122" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A123" t="s">
         <v>243</v>
       </c>
@@ -6741,8 +7305,14 @@
       <c r="E123">
         <v>16</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F123" t="s">
+        <v>6</v>
+      </c>
+      <c r="G123" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A124" t="s">
         <v>409</v>
       </c>
@@ -6758,8 +7328,14 @@
       <c r="E124">
         <v>17</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F124" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G124" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A125" t="s">
         <v>282</v>
       </c>
@@ -6775,8 +7351,14 @@
       <c r="E125">
         <v>17</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F125" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G125" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A126" t="s">
         <v>246</v>
       </c>
@@ -6792,8 +7374,14 @@
       <c r="E126">
         <v>17</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F126" t="s">
+        <v>15</v>
+      </c>
+      <c r="G126" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A127" t="s">
         <v>242</v>
       </c>
@@ -6809,8 +7397,14 @@
       <c r="E127">
         <v>18</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F127" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G127" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A128" t="s">
         <v>212</v>
       </c>
@@ -6826,8 +7420,14 @@
       <c r="E128">
         <v>20</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F128" t="s">
+        <v>6</v>
+      </c>
+      <c r="G128" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A129" t="s">
         <v>213</v>
       </c>
@@ -6843,8 +7443,14 @@
       <c r="E129">
         <v>20</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F129" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G129" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A130" t="s">
         <v>23</v>
       </c>
@@ -6860,8 +7466,14 @@
       <c r="E130">
         <v>21</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F130" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G130" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A131" t="s">
         <v>264</v>
       </c>
@@ -6877,8 +7489,14 @@
       <c r="E131">
         <v>21</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F131" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G131" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A132" t="s">
         <v>225</v>
       </c>
@@ -6894,8 +7512,14 @@
       <c r="E132">
         <v>22</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F132" t="s">
+        <v>6</v>
+      </c>
+      <c r="G132" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A133" t="s">
         <v>988</v>
       </c>
@@ -6911,8 +7535,14 @@
       <c r="E133">
         <v>22</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F133" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G133" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -6928,8 +7558,14 @@
       <c r="E134">
         <v>23</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F134" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G134" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A135" t="s">
         <v>234</v>
       </c>
@@ -6945,8 +7581,14 @@
       <c r="E135">
         <v>24</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F135" t="s">
+        <v>6</v>
+      </c>
+      <c r="G135" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A136" t="s">
         <v>980</v>
       </c>
@@ -6962,8 +7604,14 @@
       <c r="E136">
         <v>24</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F136" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G136" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A137" t="s">
         <v>240</v>
       </c>
@@ -6979,8 +7627,14 @@
       <c r="E137">
         <v>24</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F137" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G137" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A138" t="s">
         <v>289</v>
       </c>
@@ -6996,8 +7650,14 @@
       <c r="E138">
         <v>25</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F138" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G138" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A139" t="s">
         <v>244</v>
       </c>
@@ -7013,8 +7673,14 @@
       <c r="E139">
         <v>26</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F139" t="s">
+        <v>6</v>
+      </c>
+      <c r="G139" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A140" t="s">
         <v>470</v>
       </c>
@@ -7030,8 +7696,14 @@
       <c r="E140">
         <v>27</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F140" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G140" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A141" t="s">
         <v>471</v>
       </c>
@@ -7047,8 +7719,14 @@
       <c r="E141">
         <v>27</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F141" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G141" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A142" t="s">
         <v>241</v>
       </c>
@@ -7064,8 +7742,14 @@
       <c r="E142">
         <v>28</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F142" t="s">
+        <v>6</v>
+      </c>
+      <c r="G142" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A143" t="s">
         <v>287</v>
       </c>
@@ -7081,8 +7765,14 @@
       <c r="E143">
         <v>29</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F143" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G143" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A144" t="s">
         <v>233</v>
       </c>
@@ -7098,8 +7788,14 @@
       <c r="E144">
         <v>29</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F144" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G144" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A145" t="s">
         <v>485</v>
       </c>
@@ -7115,8 +7811,14 @@
       <c r="E145">
         <v>29</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F145" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G145" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A146" t="s">
         <v>204</v>
       </c>
@@ -7132,8 +7834,14 @@
       <c r="E146">
         <v>32</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F146" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G146" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A147" t="s">
         <v>515</v>
       </c>
@@ -7149,8 +7857,14 @@
       <c r="E147">
         <v>34</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F147" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G147" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A148" t="s">
         <v>537</v>
       </c>
@@ -7166,8 +7880,14 @@
       <c r="E148">
         <v>38</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F148" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G148" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A149" t="s">
         <v>211</v>
       </c>
@@ -7183,8 +7903,14 @@
       <c r="E149">
         <v>38</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F149" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G149" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A150" t="s">
         <v>962</v>
       </c>
@@ -7200,8 +7926,14 @@
       <c r="E150">
         <v>39</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F150" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G150" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A151" t="s">
         <v>218</v>
       </c>
@@ -7217,8 +7949,14 @@
       <c r="E151">
         <v>44</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F151" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G151" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A152" t="s">
         <v>583</v>
       </c>
@@ -7234,8 +7972,14 @@
       <c r="E152">
         <v>47</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F152" t="s">
+        <v>6</v>
+      </c>
+      <c r="G152" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A153" t="s">
         <v>226</v>
       </c>
@@ -7251,8 +7995,14 @@
       <c r="E153">
         <v>51</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F153" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G153" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A154" t="s">
         <v>614</v>
       </c>
@@ -7268,8 +8018,14 @@
       <c r="E154">
         <v>54</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F154" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G154" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A155" t="s">
         <v>624</v>
       </c>
@@ -7285,8 +8041,14 @@
       <c r="E155">
         <v>54</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F155" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G155" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A156" t="s">
         <v>634</v>
       </c>
@@ -7302,8 +8064,14 @@
       <c r="E156">
         <v>55</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F156" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G156" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A157" t="s">
         <v>674</v>
       </c>
@@ -7319,8 +8087,14 @@
       <c r="E157">
         <v>61</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F157" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G157" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A158" t="s">
         <v>693</v>
       </c>
@@ -7336,8 +8110,14 @@
       <c r="E158">
         <v>62</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F158" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G158" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A159" t="s">
         <v>293</v>
       </c>
@@ -7353,8 +8133,14 @@
       <c r="E159" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F159" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G159" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A160" t="s">
         <v>1399</v>
       </c>
@@ -7370,8 +8156,14 @@
       <c r="E160" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F160" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G160" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A161" t="s">
         <v>1144</v>
       </c>
@@ -7387,8 +8179,14 @@
       <c r="E161" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F161" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G161" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A162" t="s">
         <v>1207</v>
       </c>
@@ -7404,8 +8202,14 @@
       <c r="E162" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F162" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G162" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A163" t="s">
         <v>1292</v>
       </c>
@@ -7421,8 +8225,14 @@
       <c r="E163" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F163" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G163" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A164" t="s">
         <v>1064</v>
       </c>
@@ -7438,8 +8248,14 @@
       <c r="E164" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F164" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G164" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A165" t="s">
         <v>1166</v>
       </c>
@@ -7455,8 +8271,14 @@
       <c r="E165" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F165" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G165" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A166" t="s">
         <v>292</v>
       </c>
@@ -7472,8 +8294,14 @@
       <c r="E166" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F166" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G166" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A167" t="s">
         <v>1031</v>
       </c>
@@ -7489,8 +8317,14 @@
       <c r="E167" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F167" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G167" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A168" t="s">
         <v>263</v>
       </c>
@@ -7506,8 +8340,14 @@
       <c r="E168" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F168" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G168" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A169" t="s">
         <v>1400</v>
       </c>
@@ -7523,8 +8363,14 @@
       <c r="E169" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F169" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G169" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A170" t="s">
         <v>1401</v>
       </c>
@@ -7540,8 +8386,14 @@
       <c r="E170" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F170" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G170" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A171" t="s">
         <v>1085</v>
       </c>
@@ -7557,8 +8409,14 @@
       <c r="E171" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F171" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G171" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A172" t="s">
         <v>1402</v>
       </c>
@@ -7574,8 +8432,14 @@
       <c r="E172" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F172" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G172" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A173" t="s">
         <v>1092</v>
       </c>
@@ -7591,8 +8455,14 @@
       <c r="E173" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F173" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G173" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A174" t="s">
         <v>1082</v>
       </c>
@@ -7608,8 +8478,14 @@
       <c r="E174" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F174" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G174" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A175" t="s">
         <v>291</v>
       </c>
@@ -7625,8 +8501,14 @@
       <c r="E175" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F175" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G175" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A176" t="s">
         <v>1403</v>
       </c>
@@ -7642,8 +8524,14 @@
       <c r="E176" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F176" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G176" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A177" t="s">
         <v>1404</v>
       </c>
@@ -7659,8 +8547,14 @@
       <c r="E177" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F177" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G177" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A178" t="s">
         <v>1405</v>
       </c>
@@ -7676,8 +8570,14 @@
       <c r="E178" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F178" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G178" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A179" t="s">
         <v>1176</v>
       </c>
@@ -7693,8 +8593,14 @@
       <c r="E179" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F179" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G179" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A180" t="s">
         <v>1148</v>
       </c>
@@ -7710,8 +8616,14 @@
       <c r="E180" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F180" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G180" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A181" t="s">
         <v>1406</v>
       </c>
@@ -7727,8 +8639,14 @@
       <c r="E181" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F181" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G181" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A182" t="s">
         <v>1153</v>
       </c>
@@ -7744,8 +8662,14 @@
       <c r="E182" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F182" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G182" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A183" t="s">
         <v>1407</v>
       </c>
@@ -7761,8 +8685,14 @@
       <c r="E183" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F183" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G183" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A184" t="s">
         <v>1246</v>
       </c>
@@ -7778,8 +8708,14 @@
       <c r="E184" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F184" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G184" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A185" t="s">
         <v>1247</v>
       </c>
@@ -7795,8 +8731,14 @@
       <c r="E185" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F185" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G185" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A186" t="s">
         <v>278</v>
       </c>
@@ -7812,8 +8754,14 @@
       <c r="E186" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F186" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G186" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A187" t="s">
         <v>1042</v>
       </c>
@@ -7829,8 +8777,14 @@
       <c r="E187" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F187" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G187" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A188" t="s">
         <v>283</v>
       </c>
@@ -7846,8 +8800,14 @@
       <c r="E188" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F188" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G188" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A189" t="s">
         <v>273</v>
       </c>
@@ -7863,8 +8823,14 @@
       <c r="E189" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F189" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G189" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A190" t="s">
         <v>1061</v>
       </c>
@@ -7880,8 +8846,14 @@
       <c r="E190" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F190" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G190" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A191" t="s">
         <v>772</v>
       </c>
@@ -7897,8 +8869,14 @@
       <c r="E191" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F191" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G191" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A192" t="s">
         <v>1008</v>
       </c>
@@ -7914,8 +8892,14 @@
       <c r="E192" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F192" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G192" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A193" t="s">
         <v>1351</v>
       </c>
@@ -7931,8 +8915,14 @@
       <c r="E193" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F193" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G193" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A194" t="s">
         <v>220</v>
       </c>
@@ -7948,8 +8938,14 @@
       <c r="E194" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F194" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G194" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A195" t="s">
         <v>228</v>
       </c>
@@ -7965,8 +8961,14 @@
       <c r="E195" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F195" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G195" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A196" t="s">
         <v>229</v>
       </c>
@@ -7982,8 +8984,14 @@
       <c r="E196" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F196" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G196" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A197" t="s">
         <v>260</v>
       </c>
@@ -7999,8 +9007,14 @@
       <c r="E197" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F197" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G197" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A198" t="s">
         <v>286</v>
       </c>
@@ -8016,8 +9030,14 @@
       <c r="E198" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F198" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G198" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A199" t="s">
         <v>1065</v>
       </c>
@@ -8033,8 +9053,14 @@
       <c r="E199" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F199" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G199" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A200" t="s">
         <v>697</v>
       </c>
@@ -8050,8 +9076,14 @@
       <c r="E200" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F200" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G200" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A201" t="s">
         <v>629</v>
       </c>
@@ -8067,8 +9099,14 @@
       <c r="E201" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F201" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G201" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A202" t="s">
         <v>1120</v>
       </c>
@@ -8084,8 +9122,14 @@
       <c r="E202" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F202" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G202" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A203" t="s">
         <v>1041</v>
       </c>
@@ -8101,8 +9145,14 @@
       <c r="E203" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F203" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G203" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A204" t="s">
         <v>1087</v>
       </c>
@@ -8118,8 +9168,14 @@
       <c r="E204" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F204" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G204" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A205" t="s">
         <v>659</v>
       </c>
@@ -8135,8 +9191,14 @@
       <c r="E205" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F205" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G205" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A206" t="s">
         <v>756</v>
       </c>
@@ -8152,8 +9214,14 @@
       <c r="E206" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F206" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G206" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A207" t="s">
         <v>1024</v>
       </c>
@@ -8169,8 +9237,14 @@
       <c r="E207" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F207" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G207" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A208" t="s">
         <v>567</v>
       </c>
@@ -8186,8 +9260,14 @@
       <c r="E208" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F208" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G208" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A209" t="s">
         <v>247</v>
       </c>
@@ -8203,8 +9283,14 @@
       <c r="E209" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F209" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G209" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A210" t="s">
         <v>483</v>
       </c>
@@ -8220,8 +9306,14 @@
       <c r="E210" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F210" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G210" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A211" t="s">
         <v>725</v>
       </c>
@@ -8237,8 +9329,14 @@
       <c r="E211" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F211" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G211" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A212" t="s">
         <v>683</v>
       </c>
@@ -8254,8 +9352,14 @@
       <c r="E212" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="F212" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G212" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A213" t="s">
         <v>652</v>
       </c>
@@ -8271,13 +9375,15 @@
       <c r="E213" t="e">
         <v>#N/A</v>
       </c>
+      <c r="F213" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G213" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A31:E213" xr:uid="{2B159E54-99E5-4537-A261-1352C227AF32}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A32:E213">
-      <sortCondition ref="D31"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A31:G31" xr:uid="{2B159E54-99E5-4537-A261-1352C227AF32}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A32:D213">
     <sortCondition ref="D32:D213"/>
     <sortCondition descending="1" ref="B32:B213"/>

</xml_diff>